<commit_message>
added kelola user API
</commit_message>
<xml_diff>
--- a/Rekap tamu.xlsx
+++ b/Rekap tamu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>DEWAN PERWAKILAN RAKYAT DAERAH</t>
   </si>
@@ -26,7 +26,7 @@
     <t>REKAP TAMU</t>
   </si>
   <si>
-    <t>Periode2023-02-02 - 2023-07-02</t>
+    <t>Periode 2022-07-05 - 2023-06-18</t>
   </si>
   <si>
     <t>No</t>
@@ -62,15 +62,6 @@
     <t>082233659</t>
   </si>
   <si>
-    <t>2023-06-19</t>
-  </si>
-  <si>
-    <t>10:00:55</t>
-  </si>
-  <si>
-    <t>Persidangan</t>
-  </si>
-  <si>
     <t>2023-06-17</t>
   </si>
   <si>
@@ -86,12 +77,6 @@
     <t>22:54:00</t>
   </si>
   <si>
-    <t>2023-06-21</t>
-  </si>
-  <si>
-    <t>22:53:00</t>
-  </si>
-  <si>
     <t>2023-06-01</t>
   </si>
   <si>
@@ -102,18 +87,6 @@
   </si>
   <si>
     <t>Komisi-A</t>
-  </si>
-  <si>
-    <t>2023-06-30</t>
-  </si>
-  <si>
-    <t>19:38:00</t>
-  </si>
-  <si>
-    <t>Keuangan</t>
-  </si>
-  <si>
-    <t>13:26:00</t>
   </si>
 </sst>
 </file>
@@ -488,10 +461,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A12" sqref="A12:H12"/>
+      <selection activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -562,7 +535,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="2">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>17</v>
@@ -591,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -608,120 +581,16 @@
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="2">
-        <v>12</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="2">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="2">
-        <v>12</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added manage data divisi API
</commit_message>
<xml_diff>
--- a/Rekap tamu.xlsx
+++ b/Rekap tamu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>DEWAN PERWAKILAN RAKYAT DAERAH</t>
   </si>
@@ -26,7 +26,7 @@
     <t>REKAP TAMU</t>
   </si>
   <si>
-    <t>Periode 2023-06-12 - 2023-06-18</t>
+    <t>Periode 2022-03-17 - 2023-06-21</t>
   </si>
   <si>
     <t>No</t>
@@ -53,28 +53,67 @@
     <t>Tujuan Bagian</t>
   </si>
   <si>
-    <t>syahrul</t>
-  </si>
-  <si>
-    <t>Kantor Bupati Jawa Tengah</t>
+    <t xml:space="preserve">Nafisa </t>
+  </si>
+  <si>
+    <t>PT Pelita Jaya Harapann</t>
+  </si>
+  <si>
+    <t>002131618</t>
+  </si>
+  <si>
+    <t>2023-06-19</t>
+  </si>
+  <si>
+    <t>09:00:28</t>
+  </si>
+  <si>
+    <t>Umum</t>
+  </si>
+  <si>
+    <t>Nafisa Azzahra</t>
+  </si>
+  <si>
+    <t>PT Sinar Kasih</t>
   </si>
   <si>
     <t>082233659</t>
   </si>
   <si>
+    <t>Komisi C</t>
+  </si>
+  <si>
+    <t>09:00:27</t>
+  </si>
+  <si>
+    <t>Persidangan</t>
+  </si>
+  <si>
+    <t>10:00:55</t>
+  </si>
+  <si>
     <t>2023-06-17</t>
   </si>
   <si>
     <t>00:05:00</t>
   </si>
   <si>
-    <t>Umum</t>
-  </si>
-  <si>
     <t>2023-06-16</t>
   </si>
   <si>
     <t>22:54:00</t>
+  </si>
+  <si>
+    <t>2023-06-01</t>
+  </si>
+  <si>
+    <t>03:51:00</t>
+  </si>
+  <si>
+    <t>10 orang</t>
+  </si>
+  <si>
+    <t>Komisi-A</t>
   </si>
 </sst>
 </file>
@@ -449,10 +488,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A7" sqref="A7:H7"/>
+      <selection activeCell="A12" sqref="A12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -523,7 +562,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="2">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>17</v>
@@ -534,25 +573,155 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="2">
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>